<commit_message>
Updated px_cli documentation. Minor code beautification.
</commit_message>
<xml_diff>
--- a/doc/images/cli/cli.xlsx
+++ b/doc/images/cli/cli.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Work\PICONOMIX\libraries\piconomix-fwlib\trunk\doc\images\cli\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\PICONOMIX\libraries\piconomix-fwlib\doc\images\cli\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78853E0-FFDE-41AB-858C-79D1F749382E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Structures" sheetId="7" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="58">
   <si>
     <t>handler</t>
   </si>
@@ -166,9 +167,6 @@
     <t>&amp;buzzer_fn()</t>
   </si>
   <si>
-    <t>Address of function to call when command is executed</t>
-  </si>
-  <si>
     <t>Address of command structure or Address of group structure</t>
   </si>
   <si>
@@ -188,12 +186,21 @@
   </si>
   <si>
     <t>&amp;CMD_BUZZER</t>
+  </si>
+  <si>
+    <t>Address of function to call to execute command</t>
+  </si>
+  <si>
+    <t>CMD_LIST array</t>
+  </si>
+  <si>
+    <t>CMD_LIST_LED array</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -210,30 +217,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FFC0A820"/>
+      <name val="Symbol"/>
+      <family val="1"/>
+      <charset val="2"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
-      <color theme="0"/>
+      <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <color theme="0"/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFC0A820"/>
-      <name val="Symbol"/>
-      <family val="1"/>
-      <charset val="2"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -253,18 +258,30 @@
       </patternFill>
     </fill>
     <fill>
+      <patternFill patternType="lightUp">
+        <bgColor theme="0"/>
+      </patternFill>
+    </fill>
+    <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC0A820"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="lightUp">
-        <bgColor theme="0"/>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -274,16 +291,76 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFC0A820"/>
+        <color theme="1"/>
       </left>
       <right style="thin">
         <color rgb="FFC0A820"/>
       </right>
       <top style="thin">
-        <color rgb="FFC0A820"/>
+        <color theme="1"/>
       </top>
       <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFC0A820"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFC0A820"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFC0A820"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -291,25 +368,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -338,18 +425,24 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Straight Arrow Connector 2"/>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -362,7 +455,7 @@
         </a:prstGeom>
         <a:ln>
           <a:solidFill>
-            <a:srgbClr val="C0A820"/>
+            <a:schemeClr val="tx1"/>
           </a:solidFill>
           <a:tailEnd type="triangle"/>
         </a:ln>
@@ -388,18 +481,24 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>104776</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="4" name="Straight Arrow Connector 3"/>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -412,7 +511,7 @@
         </a:prstGeom>
         <a:ln>
           <a:solidFill>
-            <a:srgbClr val="C0A820"/>
+            <a:schemeClr val="tx1"/>
           </a:solidFill>
           <a:tailEnd type="triangle"/>
         </a:ln>
@@ -438,18 +537,24 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>104776</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="5" name="Straight Arrow Connector 4"/>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -462,7 +567,7 @@
         </a:prstGeom>
         <a:ln>
           <a:solidFill>
-            <a:srgbClr val="C0A820"/>
+            <a:schemeClr val="tx1"/>
           </a:solidFill>
           <a:tailEnd type="triangle"/>
         </a:ln>
@@ -488,18 +593,24 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="7" name="Straight Arrow Connector 6"/>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -512,7 +623,7 @@
         </a:prstGeom>
         <a:ln>
           <a:solidFill>
-            <a:srgbClr val="C0A820"/>
+            <a:schemeClr val="tx1"/>
           </a:solidFill>
           <a:tailEnd type="triangle"/>
         </a:ln>
@@ -538,18 +649,24 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="9" name="Straight Arrow Connector 8"/>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -562,7 +679,7 @@
         </a:prstGeom>
         <a:ln>
           <a:solidFill>
-            <a:srgbClr val="C0A820"/>
+            <a:schemeClr val="tx1"/>
           </a:solidFill>
           <a:tailEnd type="triangle"/>
         </a:ln>
@@ -588,18 +705,24 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="23" name="Straight Arrow Connector 22"/>
+        <xdr:cNvPr id="23" name="Straight Arrow Connector 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000017000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -612,7 +735,7 @@
         </a:prstGeom>
         <a:ln>
           <a:solidFill>
-            <a:srgbClr val="C0A820"/>
+            <a:schemeClr val="tx1"/>
           </a:solidFill>
           <a:tailEnd type="triangle"/>
         </a:ln>
@@ -713,6 +836,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -748,6 +888,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -923,11 +1080,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -946,33 +1103,33 @@
     </row>
     <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="9"/>
+      <c r="C2" s="13"/>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="7"/>
+      <c r="C3" s="9"/>
       <c r="D3" s="1" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" s="2"/>
     </row>
@@ -982,29 +1139,29 @@
     </row>
     <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="9"/>
+      <c r="C6" s="15"/>
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="7"/>
+      <c r="C7" s="19"/>
       <c r="D7" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="7"/>
+      <c r="C8" s="19"/>
       <c r="D8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1012,10 +1169,10 @@
     </row>
     <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="7"/>
+      <c r="C9" s="19"/>
       <c r="D9" s="1" t="s">
         <v>10</v>
       </c>
@@ -1023,23 +1180,23 @@
     </row>
     <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="7"/>
+      <c r="C10" s="19"/>
       <c r="D10" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="7"/>
+      <c r="C11" s="19"/>
       <c r="D11" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E11" s="2"/>
     </row>
@@ -1049,40 +1206,44 @@
     </row>
     <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="9"/>
+      <c r="C13" s="17"/>
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="7"/>
+      <c r="C14" s="19"/>
       <c r="D14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="7"/>
+      <c r="C15" s="19"/>
       <c r="D15" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
       <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -1104,11 +1265,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1122,7 +1283,7 @@
     <col min="9" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1136,353 +1297,378 @@
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
-    </row>
-    <row r="2" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="N1" s="2"/>
+    </row>
+    <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="20"/>
+      <c r="F2" s="21"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="21"/>
+      <c r="N2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="M2" s="2"/>
-    </row>
-    <row r="3" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="6" t="s">
+      <c r="C3" s="13"/>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="M3" s="2"/>
-    </row>
-    <row r="4" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="9"/>
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C5" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="8" t="s">
+      <c r="D5" s="3"/>
+      <c r="E5" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="M4" s="2"/>
-    </row>
-    <row r="5" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="8" t="s">
+      <c r="F5" s="17"/>
+      <c r="N5" s="2"/>
+    </row>
+    <row r="6" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="E5" s="6" t="s">
+      <c r="C6" s="13"/>
+      <c r="E6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="7"/>
-      <c r="M5" s="2"/>
-    </row>
-    <row r="6" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="6" t="s">
+      <c r="F6" s="5"/>
+      <c r="H6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="N6" s="2"/>
+    </row>
+    <row r="7" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="E6" s="6" t="s">
+      <c r="C7" s="9"/>
+      <c r="E7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="8" t="s">
+      <c r="F7" s="5"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="I6" s="9"/>
-      <c r="M6" s="2"/>
-    </row>
-    <row r="7" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="I7" s="13"/>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="7"/>
-      <c r="M7" s="2"/>
-    </row>
-    <row r="8" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="8" t="s">
+      <c r="I8" s="9"/>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="E8" s="8" t="s">
+      <c r="C9" s="13"/>
+      <c r="E9" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="9"/>
-      <c r="H8" s="3" t="s">
+      <c r="F9" s="15"/>
+      <c r="H9" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I9" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="J8" s="5"/>
-      <c r="K8" s="8" t="s">
+      <c r="J9" s="3"/>
+      <c r="K9" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="L8" s="9"/>
-      <c r="M8" s="2"/>
-    </row>
-    <row r="9" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="6" t="s">
+      <c r="L9" s="15"/>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="E9" s="6" t="s">
+      <c r="C10" s="9"/>
+      <c r="E10" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="7"/>
-      <c r="H9" s="8" t="s">
+      <c r="F10" s="5"/>
+      <c r="H10" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="I9" s="9"/>
-      <c r="K9" s="6" t="s">
+      <c r="I10" s="13"/>
+      <c r="K10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L9" s="7"/>
-      <c r="M9" s="2"/>
-    </row>
-    <row r="10" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="3" t="s">
+      <c r="L10" s="5"/>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C11" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E11" s="6">
         <v>1</v>
       </c>
-      <c r="F10" s="11"/>
-      <c r="H10" s="6" t="s">
+      <c r="F11" s="7"/>
+      <c r="H11" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="I10" s="7"/>
-      <c r="K10" s="10">
+      <c r="I11" s="9"/>
+      <c r="K11" s="6">
         <v>0</v>
       </c>
-      <c r="L10" s="11"/>
-      <c r="M10" s="2"/>
-    </row>
-    <row r="11" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="8" t="s">
+      <c r="L11" s="7"/>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="9"/>
-      <c r="E11" s="10">
+      <c r="C12" s="13"/>
+      <c r="E12" s="6">
         <v>1</v>
       </c>
-      <c r="F11" s="11"/>
-      <c r="H11" s="3" t="s">
+      <c r="F12" s="7"/>
+      <c r="H12" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I12" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="K11" s="10">
+      <c r="K12" s="6">
         <v>0</v>
       </c>
-      <c r="L11" s="11"/>
-      <c r="M11" s="2"/>
-    </row>
-    <row r="12" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="6" t="s">
+      <c r="L12" s="7"/>
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="E12" s="6" t="s">
+      <c r="C13" s="9"/>
+      <c r="E13" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="7"/>
-      <c r="H12" s="8" t="s">
+      <c r="F13" s="5"/>
+      <c r="H13" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="I12" s="9"/>
-      <c r="K12" s="6" t="s">
+      <c r="I13" s="13"/>
+      <c r="K13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="L12" s="7"/>
-      <c r="M12" s="2"/>
-    </row>
-    <row r="13" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="3" t="s">
+      <c r="L13" s="5"/>
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C14" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E14" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="7"/>
-      <c r="H13" s="6" t="s">
+      <c r="F14" s="5"/>
+      <c r="H14" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I13" s="7"/>
-      <c r="K13" s="6" t="s">
+      <c r="I14" s="9"/>
+      <c r="K14" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L13" s="7"/>
-      <c r="M13" s="2"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
-      <c r="H14" s="3" t="s">
+      <c r="L14" s="5"/>
+      <c r="N14" s="2"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="2"/>
+      <c r="H15" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="I15" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="M14" s="2"/>
-    </row>
-    <row r="15" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="E15" s="8" t="s">
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="E16" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="9"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="8" t="s">
+      <c r="F16" s="15"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="L15" s="9"/>
-      <c r="M15" s="2"/>
-    </row>
-    <row r="16" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="E16" s="6" t="s">
+      <c r="L16" s="15"/>
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="E17" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="7"/>
-      <c r="K16" s="6" t="s">
+      <c r="F17" s="5"/>
+      <c r="K17" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L16" s="7"/>
-      <c r="M16" s="2"/>
-    </row>
-    <row r="17" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="E17" s="10">
+      <c r="L17" s="5"/>
+      <c r="N17" s="2"/>
+    </row>
+    <row r="18" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="E18" s="6">
         <v>0</v>
       </c>
-      <c r="F17" s="11"/>
-      <c r="K17" s="10">
+      <c r="F18" s="7"/>
+      <c r="K18" s="6">
         <v>0</v>
       </c>
-      <c r="L17" s="11"/>
-      <c r="M17" s="2"/>
-    </row>
-    <row r="18" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="E18" s="10">
+      <c r="L18" s="7"/>
+      <c r="N18" s="2"/>
+    </row>
+    <row r="19" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="E19" s="6">
         <v>1</v>
       </c>
-      <c r="F18" s="11"/>
-      <c r="K18" s="10">
+      <c r="F19" s="7"/>
+      <c r="K19" s="6">
         <v>0</v>
       </c>
-      <c r="L18" s="11"/>
-      <c r="M18" s="2"/>
-    </row>
-    <row r="19" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="E19" s="6" t="s">
+      <c r="L19" s="7"/>
+      <c r="N19" s="2"/>
+    </row>
+    <row r="20" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="E20" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F19" s="7"/>
-      <c r="K19" s="6" t="s">
+      <c r="F20" s="5"/>
+      <c r="K20" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="L19" s="7"/>
-      <c r="M19" s="2"/>
-    </row>
-    <row r="20" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="E20" s="6" t="s">
+      <c r="L20" s="5"/>
+      <c r="N20" s="2"/>
+    </row>
+    <row r="21" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="E21" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F20" s="7"/>
-      <c r="K20" s="6" t="s">
+      <c r="F21" s="5"/>
+      <c r="K21" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="L20" s="7"/>
-      <c r="M20" s="2"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
+      <c r="L21" s="5"/>
+      <c r="N21" s="2"/>
+    </row>
+    <row r="22" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="21"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="21"/>
+      <c r="N22" s="2"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="B6:C6"/>
     <mergeCell ref="K16:L16"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="H6:I6"/>
     <mergeCell ref="H7:I7"/>
-    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="H8:I8"/>
     <mergeCell ref="K9:L9"/>
     <mergeCell ref="K10:L10"/>
     <mergeCell ref="K11:L11"/>
     <mergeCell ref="K12:L12"/>
     <mergeCell ref="K13:L13"/>
-    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="K14:L14"/>
     <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H11:I11"/>
     <mergeCell ref="H13:I13"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>